<commit_message>
PWL_POS: stok change user_id to supplier_id
</commit_message>
<xml_diff>
--- a/Semester-4/WebLanjut/PWL_POS/public/template_data/stok.xlsx
+++ b/Semester-4/WebLanjut/PWL_POS/public/template_data/stok.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\Polinema\Polinema.task\Semester-4\WebLanjut\PWL_POS\public\template_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34039E85-B546-4FEB-8D24-74C54B555FBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E34C9F98-EFBB-47E4-BA38-F90455E5C099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,9 +25,6 @@
     <t>ID Barang</t>
   </si>
   <si>
-    <t>ID User</t>
-  </si>
-  <si>
     <t>Tanggal Stok</t>
   </si>
   <si>
@@ -35,6 +32,9 @@
   </si>
   <si>
     <t>2025-04-08 12:20:05</t>
+  </si>
+  <si>
+    <t>ID Supplier</t>
   </si>
 </sst>
 </file>
@@ -384,7 +384,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -400,13 +400,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -417,7 +417,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2">
         <v>158</v>
@@ -431,7 +431,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D3">
         <v>210</v>
@@ -445,7 +445,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4">
         <v>77</v>
@@ -459,7 +459,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5">
         <v>60</v>
@@ -473,7 +473,7 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D6">
         <v>243</v>
@@ -487,7 +487,7 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D7">
         <v>127</v>
@@ -501,7 +501,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D8">
         <v>115</v>
@@ -515,7 +515,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9">
         <v>222</v>
@@ -529,7 +529,7 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10">
         <v>225</v>
@@ -543,7 +543,7 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D11">
         <v>58</v>

</xml_diff>